<commit_message>
Correct Tm and Tl in Sputter Sheet
</commit_message>
<xml_diff>
--- a/MgZnCa - Charge Calcs Notes.xlsx
+++ b/MgZnCa - Charge Calcs Notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="At% to Wt%" sheetId="1" state="hidden" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="264">
   <si>
     <t>Mg</t>
   </si>
@@ -663,9 +663,6 @@
     <t>Jake Thesis</t>
   </si>
   <si>
-    <t>Jake has about 400C</t>
-  </si>
-  <si>
     <t>xx</t>
   </si>
   <si>
@@ -841,6 +838,12 @@
   </si>
   <si>
     <t>Area [h/2*(t0+tn)]</t>
+  </si>
+  <si>
+    <t>Tl</t>
+  </si>
+  <si>
+    <t>Jake Paper</t>
   </si>
 </sst>
 </file>
@@ -2919,10 +2922,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="121" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J1" s="121" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
@@ -4973,7 +4976,7 @@
       <c r="L51" s="197"/>
       <c r="M51" s="197"/>
       <c r="N51" s="197" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O51" s="197" t="s">
         <v>198</v>
@@ -5027,7 +5030,7 @@
       <c r="L53" s="191"/>
       <c r="M53" s="191"/>
       <c r="N53" s="191" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O53" s="191"/>
       <c r="P53" s="191"/>
@@ -5054,7 +5057,7 @@
       <c r="L54" s="191"/>
       <c r="M54" s="191"/>
       <c r="N54" s="191" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O54" s="191"/>
       <c r="P54" s="191"/>
@@ -5110,7 +5113,7 @@
       <c r="L56" s="191"/>
       <c r="M56" s="191"/>
       <c r="N56" s="191" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O56" s="191"/>
       <c r="P56" s="191"/>
@@ -5140,7 +5143,7 @@
       <c r="M57" s="191"/>
       <c r="N57" s="191"/>
       <c r="O57" s="191" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P57" s="191"/>
       <c r="Q57" s="191"/>
@@ -5169,7 +5172,7 @@
       <c r="M58" s="191"/>
       <c r="N58" s="191"/>
       <c r="O58" s="191" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P58" s="191"/>
       <c r="Q58" s="191"/>
@@ -5249,7 +5252,7 @@
       <c r="L61" s="191"/>
       <c r="M61" s="191"/>
       <c r="N61" s="191" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O61" s="191"/>
       <c r="P61" s="191"/>
@@ -5279,7 +5282,7 @@
       <c r="M62" s="191"/>
       <c r="N62" s="191"/>
       <c r="O62" s="191" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P62" s="191"/>
       <c r="Q62" s="191"/>
@@ -5308,7 +5311,7 @@
       <c r="M63" s="191"/>
       <c r="N63" s="191"/>
       <c r="O63" s="191" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P63" s="191"/>
       <c r="Q63" s="191"/>
@@ -5337,7 +5340,7 @@
       <c r="M64" s="191"/>
       <c r="N64" s="191"/>
       <c r="O64" s="191" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P64" s="191"/>
       <c r="Q64" s="191"/>
@@ -5364,7 +5367,7 @@
       <c r="M65" s="191"/>
       <c r="N65" s="191"/>
       <c r="O65" s="191" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P65" s="191"/>
       <c r="Q65" s="191"/>
@@ -5446,7 +5449,7 @@
       <c r="L68" s="191"/>
       <c r="M68" s="191"/>
       <c r="N68" s="191" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O68" s="191"/>
       <c r="P68" s="191"/>
@@ -5476,7 +5479,7 @@
       <c r="M69" s="191"/>
       <c r="N69" s="191"/>
       <c r="O69" s="191" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P69" s="191"/>
       <c r="Q69" s="191"/>
@@ -5911,10 +5914,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="121" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J1" s="121" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
@@ -7951,7 +7954,7 @@
       <c r="L51" s="197"/>
       <c r="M51" s="197"/>
       <c r="N51" s="197" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O51" s="197" t="s">
         <v>198</v>
@@ -8005,7 +8008,7 @@
       <c r="L53" s="191"/>
       <c r="M53" s="191"/>
       <c r="N53" s="191" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O53" s="191"/>
       <c r="P53" s="191"/>
@@ -8032,7 +8035,7 @@
       <c r="L54" s="191"/>
       <c r="M54" s="191"/>
       <c r="N54" s="191" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O54" s="191"/>
       <c r="P54" s="191"/>
@@ -8088,7 +8091,7 @@
       <c r="L56" s="191"/>
       <c r="M56" s="191"/>
       <c r="N56" s="191" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O56" s="191"/>
       <c r="P56" s="191"/>
@@ -8118,7 +8121,7 @@
       <c r="M57" s="191"/>
       <c r="N57" s="191"/>
       <c r="O57" s="191" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P57" s="191"/>
       <c r="Q57" s="191"/>
@@ -8173,7 +8176,7 @@
       <c r="L59" s="191"/>
       <c r="M59" s="191"/>
       <c r="N59" s="191" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O59" s="191"/>
       <c r="P59" s="191"/>
@@ -8201,7 +8204,7 @@
       <c r="M60" s="191"/>
       <c r="N60" s="197"/>
       <c r="O60" s="197" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P60" s="191"/>
       <c r="Q60" s="191"/>
@@ -8877,13 +8880,13 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="121" t="s">
+        <v>254</v>
+      </c>
+      <c r="J1" s="121" t="s">
+        <v>253</v>
+      </c>
+      <c r="M1" s="121" t="s">
         <v>255</v>
-      </c>
-      <c r="J1" s="121" t="s">
-        <v>254</v>
-      </c>
-      <c r="M1" s="121" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
@@ -10695,7 +10698,7 @@
       <c r="U43" s="191"/>
       <c r="V43" s="191"/>
       <c r="W43" s="192" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -10724,7 +10727,7 @@
       <c r="U44" s="191"/>
       <c r="V44" s="191"/>
       <c r="W44" s="192" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -10912,7 +10915,7 @@
       <c r="J51" s="197"/>
       <c r="K51" s="197"/>
       <c r="N51" s="197" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O51" s="197" t="s">
         <v>198</v>
@@ -10970,7 +10973,7 @@
       <c r="L53" s="191"/>
       <c r="M53" s="191"/>
       <c r="N53" s="191" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O53" s="191"/>
       <c r="P53" s="191"/>
@@ -10999,7 +11002,7 @@
       <c r="L54" s="191"/>
       <c r="M54" s="191"/>
       <c r="N54" s="191" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O54" s="191"/>
       <c r="P54" s="191"/>
@@ -11059,7 +11062,7 @@
       <c r="L56" s="191"/>
       <c r="M56" s="191"/>
       <c r="N56" s="191" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O56" s="191"/>
       <c r="P56" s="191"/>
@@ -11091,7 +11094,7 @@
       <c r="M57" s="191"/>
       <c r="N57" s="191"/>
       <c r="O57" s="191" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P57" s="191"/>
       <c r="Q57" s="191"/>
@@ -11122,7 +11125,7 @@
       <c r="M58" s="191"/>
       <c r="N58" s="191"/>
       <c r="O58" s="191" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P58" s="191"/>
       <c r="Q58" s="191"/>
@@ -11204,7 +11207,7 @@
       <c r="L61" s="191"/>
       <c r="M61" s="191"/>
       <c r="N61" s="191" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O61" s="191"/>
       <c r="P61" s="191"/>
@@ -11234,7 +11237,7 @@
       <c r="M62" s="191"/>
       <c r="N62" s="191"/>
       <c r="O62" s="191" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P62" s="191"/>
       <c r="Q62" s="191"/>
@@ -11263,7 +11266,7 @@
       <c r="M63" s="191"/>
       <c r="N63" s="191"/>
       <c r="O63" s="191" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P63" s="191"/>
       <c r="Q63" s="191"/>
@@ -11292,7 +11295,7 @@
       <c r="M64" s="191"/>
       <c r="N64" s="191"/>
       <c r="O64" s="191" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P64" s="191"/>
       <c r="Q64" s="191"/>
@@ -11319,7 +11322,7 @@
       <c r="M65" s="191"/>
       <c r="N65" s="191"/>
       <c r="O65" s="191" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P65" s="191"/>
       <c r="Q65" s="191"/>
@@ -11401,7 +11404,7 @@
       <c r="L68" s="191"/>
       <c r="M68" s="191"/>
       <c r="N68" s="191" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O68" s="191"/>
       <c r="P68" s="191"/>
@@ -11431,7 +11434,7 @@
       <c r="M69" s="191"/>
       <c r="N69" s="191"/>
       <c r="O69" s="191" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P69" s="191"/>
       <c r="Q69" s="191"/>
@@ -11502,7 +11505,7 @@
       <c r="G72" s="191"/>
       <c r="H72" s="191"/>
       <c r="I72" s="290" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J72" s="290"/>
       <c r="K72" s="290"/>
@@ -11525,7 +11528,7 @@
       <c r="H73" s="191"/>
       <c r="I73" s="290"/>
       <c r="J73" s="290" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K73" s="290"/>
       <c r="Q73" s="191"/>
@@ -11547,7 +11550,7 @@
       <c r="H74" s="191"/>
       <c r="I74" s="290"/>
       <c r="J74" s="290" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K74" s="290"/>
       <c r="Q74" s="191"/>
@@ -11569,7 +11572,7 @@
       <c r="H75" s="191"/>
       <c r="I75" s="290"/>
       <c r="J75" s="290" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K75" s="290"/>
       <c r="Q75" s="191"/>
@@ -11592,7 +11595,7 @@
       <c r="I76" s="290"/>
       <c r="J76" s="290"/>
       <c r="K76" s="290" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q76" s="191"/>
       <c r="R76" s="191"/>
@@ -11854,7 +11857,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
@@ -13853,7 +13856,7 @@
       <c r="J51" s="197"/>
       <c r="K51" s="197"/>
       <c r="N51" s="197" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O51" s="197" t="s">
         <v>198</v>
@@ -13907,7 +13910,7 @@
       <c r="L53" s="191"/>
       <c r="M53" s="191"/>
       <c r="N53" s="191" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O53" s="191"/>
       <c r="P53" s="191"/>
@@ -13934,7 +13937,7 @@
       <c r="L54" s="191"/>
       <c r="M54" s="191"/>
       <c r="N54" s="191" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O54" s="191"/>
       <c r="P54" s="191"/>
@@ -13990,7 +13993,7 @@
       <c r="L56" s="191"/>
       <c r="M56" s="191"/>
       <c r="N56" s="191" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O56" s="191"/>
       <c r="P56" s="191"/>
@@ -14020,7 +14023,7 @@
       <c r="M57" s="191"/>
       <c r="N57" s="191"/>
       <c r="O57" s="191" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P57" s="191"/>
       <c r="Q57" s="191"/>
@@ -14049,7 +14052,7 @@
       <c r="M58" s="191"/>
       <c r="N58" s="191"/>
       <c r="O58" s="191" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P58" s="191"/>
       <c r="Q58" s="191"/>
@@ -14129,7 +14132,7 @@
       <c r="L61" s="191"/>
       <c r="M61" s="191"/>
       <c r="N61" s="191" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O61" s="191"/>
       <c r="P61" s="191"/>
@@ -14159,7 +14162,7 @@
       <c r="M62" s="191"/>
       <c r="N62" s="191"/>
       <c r="O62" s="191" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P62" s="191"/>
       <c r="Q62" s="191"/>
@@ -14188,7 +14191,7 @@
       <c r="M63" s="191"/>
       <c r="N63" s="191"/>
       <c r="O63" s="191" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P63" s="191"/>
       <c r="Q63" s="191"/>
@@ -14217,7 +14220,7 @@
       <c r="M64" s="191"/>
       <c r="N64" s="191"/>
       <c r="O64" s="191" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P64" s="191"/>
       <c r="Q64" s="191"/>
@@ -14244,7 +14247,7 @@
       <c r="M65" s="191"/>
       <c r="N65" s="191"/>
       <c r="O65" s="191" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P65" s="191"/>
       <c r="Q65" s="191"/>
@@ -14326,7 +14329,7 @@
       <c r="L68" s="191"/>
       <c r="M68" s="191"/>
       <c r="N68" s="191" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O68" s="191"/>
       <c r="P68" s="191"/>
@@ -14356,7 +14359,7 @@
       <c r="M69" s="191"/>
       <c r="N69" s="191"/>
       <c r="O69" s="191" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P69" s="191"/>
       <c r="Q69" s="191"/>
@@ -15156,7 +15159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -15170,34 +15173,34 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="271" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="276" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="259"/>
       <c r="C3" s="259" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D3" s="260" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="263"/>
       <c r="B4" s="261"/>
       <c r="C4" s="261" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D4" s="262" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="264" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B5" s="3">
         <v>85</v>
@@ -15211,7 +15214,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="264" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="257">
@@ -15225,7 +15228,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="264" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="257">
@@ -15239,7 +15242,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="263" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="274">
@@ -15253,7 +15256,7 @@
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="276" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -15266,24 +15269,24 @@
       <c r="A11" s="263"/>
       <c r="B11" s="8"/>
       <c r="C11" s="261" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="261" t="s">
         <v>229</v>
       </c>
-      <c r="D11" s="261" t="s">
-        <v>230</v>
-      </c>
       <c r="E11" s="261" t="s">
+        <v>235</v>
+      </c>
+      <c r="F11" s="261" t="s">
         <v>236</v>
       </c>
-      <c r="F11" s="261" t="s">
+      <c r="G11" s="262" t="s">
         <v>237</v>
-      </c>
-      <c r="G11" s="262" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="264" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B12" s="3">
         <v>102</v>
@@ -15306,7 +15309,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="264" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B13" s="3">
         <v>49</v>
@@ -15319,7 +15322,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="264" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" s="3">
         <f>B12*B13</f>
@@ -15333,7 +15336,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="264" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -15359,7 +15362,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="263" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="272">
@@ -15385,53 +15388,53 @@
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="276" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="259" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="259" t="s">
         <v>228</v>
       </c>
-      <c r="D18" s="259" t="s">
+      <c r="E18" s="259" t="s">
         <v>229</v>
       </c>
-      <c r="E18" s="259" t="s">
-        <v>230</v>
-      </c>
       <c r="F18" s="259" t="s">
+        <v>235</v>
+      </c>
+      <c r="G18" s="259" t="s">
         <v>236</v>
       </c>
-      <c r="G18" s="259" t="s">
+      <c r="H18" s="260" t="s">
         <v>237</v>
-      </c>
-      <c r="H18" s="260" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="263"/>
       <c r="B19" s="8"/>
       <c r="C19" s="265" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D19" s="265" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E19" s="265" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F19" s="265" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G19" s="265" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H19" s="266" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="264" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B20" s="3">
         <v>102</v>
@@ -15457,7 +15460,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="264" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B21" s="3">
         <v>18</v>
@@ -15471,7 +15474,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="264" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -15498,7 +15501,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="264" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -15525,7 +15528,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="263" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -15552,7 +15555,7 @@
     </row>
     <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="277" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -15563,19 +15566,19 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="270"/>
       <c r="B27" s="261" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="261" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="261" t="s">
-        <v>230</v>
-      </c>
       <c r="D27" s="261" t="s">
+        <v>235</v>
+      </c>
+      <c r="E27" s="261" t="s">
         <v>236</v>
       </c>
-      <c r="E27" s="261" t="s">
+      <c r="F27" s="262" t="s">
         <v>237</v>
-      </c>
-      <c r="F27" s="262" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -15598,7 +15601,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="268" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B29" s="3">
         <f>C16</f>
@@ -15623,7 +15626,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="264" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B30" s="3">
         <f>D24</f>
@@ -17111,10 +17114,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17198,142 +17201,151 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>262</v>
       </c>
       <c r="B11">
-        <v>390</v>
+        <v>412</v>
       </c>
       <c r="C11">
         <f>B11+273.15</f>
-        <v>663.15</v>
+        <v>685.15</v>
       </c>
       <c r="D11" t="s">
+        <v>263</v>
+      </c>
+      <c r="F11" t="s">
         <v>202</v>
-      </c>
-      <c r="F11" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12">
-        <v>147</v>
+        <v>335</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C13" si="0">B12+273.15</f>
-        <v>420.15</v>
+        <f>B12+273.15</f>
+        <v>608.15</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>147</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C14" si="0">B13+273.15</f>
+        <v>420.15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>132</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>405.15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14">
-        <f>C14-273</f>
-        <v>10.604999999999961</v>
-      </c>
-      <c r="C14">
-        <f>C13*0.7</f>
-        <v>283.60499999999996</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <f>C15-273</f>
+        <v>10.604999999999961</v>
+      </c>
+      <c r="C15">
+        <f>C14*0.7</f>
+        <v>283.60499999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16">
+        <f>C16-273</f>
         <v>51.120000000000005</v>
       </c>
-      <c r="C15">
-        <f>C13*0.8</f>
+      <c r="C16">
+        <f>C14*0.8</f>
         <v>324.12</v>
       </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="84" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="84" t="s">
+      <c r="C19" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="84" t="s">
+      <c r="D19" s="84" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19">
-        <v>20</v>
-      </c>
-      <c r="C19">
-        <f>273.15+B19</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D19" s="235">
-        <f>C19/C13</f>
-        <v>0.7235591756139701</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <f>273.15+B20</f>
+        <v>293.14999999999998</v>
       </c>
       <c r="D20" s="235">
-        <f>C20/C13</f>
-        <v>4.9364432926076764E-2</v>
+        <f>C20/C14</f>
+        <v>0.7235591756139701</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="235">
+        <f>C21/C14</f>
+        <v>4.9364432926076764E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>154</v>
       </c>
-      <c r="B21">
-        <f>C21-273.15</f>
+      <c r="B22">
+        <f>C22-273.15</f>
         <v>40</v>
       </c>
-      <c r="C21">
-        <f>C19+C20</f>
+      <c r="C22">
+        <f>C20+C21</f>
         <v>313.14999999999998</v>
       </c>
-      <c r="D21" s="235">
-        <f>C21/C13</f>
+      <c r="D22" s="235">
+        <f>C22/C14</f>
         <v>0.77292360854004694</v>
       </c>
     </row>
@@ -22978,7 +22990,7 @@
         <v>196</v>
       </c>
       <c r="J1" s="121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
@@ -25807,10 +25819,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="121" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J1" s="121" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
@@ -27867,7 +27879,7 @@
       <c r="L51" s="197"/>
       <c r="M51" s="197"/>
       <c r="N51" s="197" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O51" s="197" t="s">
         <v>198</v>
@@ -27921,7 +27933,7 @@
       <c r="L53" s="191"/>
       <c r="M53" s="191"/>
       <c r="N53" s="191" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O53" s="191"/>
       <c r="P53" s="191"/>
@@ -27948,7 +27960,7 @@
       <c r="L54" s="191"/>
       <c r="M54" s="191"/>
       <c r="N54" s="191" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O54" s="191"/>
       <c r="P54" s="191"/>
@@ -28004,7 +28016,7 @@
       <c r="L56" s="191"/>
       <c r="M56" s="191"/>
       <c r="N56" s="191" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O56" s="191"/>
       <c r="P56" s="191"/>
@@ -28034,7 +28046,7 @@
       <c r="M57" s="191"/>
       <c r="N57" s="191"/>
       <c r="O57" s="191" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P57" s="191"/>
       <c r="Q57" s="191"/>
@@ -28063,7 +28075,7 @@
       <c r="M58" s="191"/>
       <c r="N58" s="191"/>
       <c r="O58" s="191" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P58" s="191"/>
       <c r="Q58" s="191"/>
@@ -28143,7 +28155,7 @@
       <c r="L61" s="191"/>
       <c r="M61" s="191"/>
       <c r="N61" s="191" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O61" s="191"/>
       <c r="P61" s="191"/>
@@ -28173,7 +28185,7 @@
       <c r="M62" s="191"/>
       <c r="N62" s="191"/>
       <c r="O62" s="191" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P62" s="191"/>
       <c r="Q62" s="191"/>
@@ -28202,7 +28214,7 @@
       <c r="M63" s="191"/>
       <c r="N63" s="191"/>
       <c r="O63" s="191" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P63" s="191"/>
       <c r="Q63" s="191"/>
@@ -28231,7 +28243,7 @@
       <c r="M64" s="191"/>
       <c r="N64" s="191"/>
       <c r="O64" s="191" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P64" s="191"/>
       <c r="Q64" s="191"/>
@@ -28258,7 +28270,7 @@
       <c r="M65" s="191"/>
       <c r="N65" s="191"/>
       <c r="O65" s="191" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P65" s="191"/>
       <c r="Q65" s="191"/>

</xml_diff>